<commit_message>
Ajouter tache dans document word et excel
</commit_message>
<xml_diff>
--- a/Feuille_de_temps_S1-Eq1.xlsx
+++ b/Feuille_de_temps_S1-Eq1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/90b80275017569d9/Documents/New folder/All-Nighter-s/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bdebqcca-my.sharepoint.com/personal/2235096_bdeb_qc_ca/Documents/Session 4/Application Web Transanctionnelles/All-Nighter-s/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{60B6172D-1160-436E-9B7C-28D73653807E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{026D9E8B-5815-40CD-B190-01BE9DD78238}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{60B6172D-1160-436E-9B7C-28D73653807E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2C15258-C79A-4617-BDF3-CDB1DE215735}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="35">
   <si>
     <t>Temps</t>
   </si>
@@ -136,6 +136,15 @@
   </si>
   <si>
     <t>Manbir</t>
+  </si>
+  <si>
+    <t>10h</t>
+  </si>
+  <si>
+    <t>24h</t>
+  </si>
+  <si>
+    <t>14h</t>
   </si>
 </sst>
 </file>
@@ -593,7 +602,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -627,7 +636,9 @@
       <c r="A3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -637,7 +648,9 @@
       <c r="A4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -647,7 +660,9 @@
       <c r="A5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -657,7 +672,9 @@
       <c r="A6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="9"/>
+      <c r="B6" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -675,7 +692,9 @@
       <c r="A9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="6">
+        <v>8</v>
+      </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -685,7 +704,9 @@
       <c r="A10" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="9"/>
+      <c r="B10" s="9">
+        <v>8</v>
+      </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -695,7 +716,9 @@
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="6">
+        <v>7</v>
+      </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -705,7 +728,9 @@
       <c r="A12" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="9"/>
+      <c r="B12" s="9">
+        <v>6</v>
+      </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>

</xml_diff>

<commit_message>
Correction mineure sur Word et Excel
</commit_message>
<xml_diff>
--- a/Feuille_de_temps_S1-Eq1.xlsx
+++ b/Feuille_de_temps_S1-Eq1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AznGa\Documents\GitHub\All-Nighter-s\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E312346E-B16D-4A95-AC81-30A2EEB9B0A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9D19E0-605B-4822-B080-49A038E2CCEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -231,9 +231,6 @@
     <t>Correction du Word</t>
   </si>
   <si>
-    <t>Petite carousel à la page d'accueil</t>
-  </si>
-  <si>
     <t>Amélioration des styles de la page de Contact</t>
   </si>
   <si>
@@ -253,9 +250,6 @@
   </si>
   <si>
     <t>Exigence non fonctionnelle dans Word</t>
-  </si>
-  <si>
-    <t>Aide dans la petite carousel dans la page d'accueil</t>
   </si>
   <si>
     <t>Écrire le README.md</t>
@@ -307,6 +301,12 @@
   </si>
   <si>
     <t>Correction + Ajout des élément du Word</t>
+  </si>
+  <si>
+    <t>Correction de Word (Petite changement)</t>
+  </si>
+  <si>
+    <t>Aide en back-end pour la page de connection (Erreur de connection ou connection réussi)</t>
   </si>
 </sst>
 </file>
@@ -780,7 +780,7 @@
   </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -975,8 +975,8 @@
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1035,16 +1035,16 @@
         <v>1</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I2" s="16">
         <v>0.5</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="C3" s="13">
         <v>2</v>
       </c>
@@ -1061,14 +1061,16 @@
         <v>0.5</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" s="16"/>
+        <v>64</v>
+      </c>
+      <c r="I3" s="16">
+        <v>0.5</v>
+      </c>
       <c r="J3" s="17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="C4" s="13">
         <v>1</v>
       </c>
@@ -1085,10 +1087,14 @@
         <v>1</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
+        <v>65</v>
+      </c>
+      <c r="I4" s="16">
+        <v>1</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C5" s="13">
@@ -1107,7 +1113,7 @@
         <v>4</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I5" s="16"/>
       <c r="J5" s="16"/>
@@ -1125,7 +1131,7 @@
         <v>0.5</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
@@ -1135,7 +1141,7 @@
         <v>1.5</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -1143,7 +1149,7 @@
         <v>0.5</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
@@ -1151,7 +1157,7 @@
         <v>2</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1232,13 +1238,13 @@
         <v>1</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I2" s="16">
         <v>2</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
@@ -1264,13 +1270,13 @@
         <v>3</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I3" s="16">
         <v>1.5</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
@@ -1296,7 +1302,7 @@
         <v>2</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I4" s="16"/>
       <c r="J4" s="16"/>
@@ -1320,7 +1326,7 @@
         <v>1.5</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I5" s="16"/>
       <c r="J5" s="16"/>
@@ -1336,7 +1342,7 @@
         <v>2.5</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
@@ -1498,7 +1504,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1625,9 +1631,7 @@
         <v>59</v>
       </c>
       <c r="I4" s="15"/>
-      <c r="J4" s="13" t="s">
-        <v>63</v>
-      </c>
+      <c r="J4" s="13"/>
     </row>
     <row r="5" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="15"/>
@@ -1666,7 +1670,7 @@
         <v>0.5</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I6" s="15"/>
       <c r="J6" s="13"/>
@@ -1679,7 +1683,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J7" s="11"/>
     </row>
@@ -8712,13 +8716,13 @@
         <v>2</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I2" s="16">
         <v>1</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="51" x14ac:dyDescent="0.2">
@@ -8740,7 +8744,7 @@
         <v>3</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
@@ -8764,7 +8768,7 @@
         <v>2</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I4" s="16"/>
       <c r="J4" s="16"/>
@@ -8784,7 +8788,7 @@
         <v>2</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I5" s="16"/>
       <c r="J5" s="16"/>
@@ -8794,7 +8798,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>

</xml_diff>

<commit_message>
page admin fixer le nav bar
</commit_message>
<xml_diff>
--- a/Feuille_de_temps_S1-Eq1.xlsx
+++ b/Feuille_de_temps_S1-Eq1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AznGa\OneDrive\Documents\GitHub\All-Nighter-s\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bdebqcca-my.sharepoint.com/personal/2235096_bdeb_qc_ca/Documents/Session 4/Application Web Transanctionnelles/All-Nighter-s/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9BD457-F2ED-4FC9-807C-1A231AC18EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{DA9BD457-F2ED-4FC9-807C-1A231AC18EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EBB6FB4-F8BF-4190-BB85-CFEE8564723E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="154">
   <si>
     <t>Temps</t>
   </si>
@@ -499,6 +499,9 @@
   </si>
   <si>
     <t>Email pas similaire</t>
+  </si>
+  <si>
+    <t>Ameliorer drop down</t>
   </si>
 </sst>
 </file>
@@ -1201,7 +1204,7 @@
       </c>
       <c r="M5" s="6">
         <f>SUM(Marc!W2:W7)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.25">
@@ -3243,7 +3246,7 @@
   </sheetPr>
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
@@ -3394,7 +3397,9 @@
       <c r="V2" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="W2" s="16"/>
+      <c r="W2" s="16">
+        <v>4</v>
+      </c>
       <c r="X2" s="16" t="s">
         <v>149</v>
       </c>
@@ -3472,7 +3477,9 @@
       <c r="V3" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="W3" s="16"/>
+      <c r="W3" s="16">
+        <v>4</v>
+      </c>
       <c r="X3" s="16" t="s">
         <v>150</v>
       </c>
@@ -3522,8 +3529,12 @@
       <c r="V4" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
+      <c r="W4" s="16">
+        <v>1</v>
+      </c>
+      <c r="X4" s="16" t="s">
+        <v>153</v>
+      </c>
       <c r="Y4" s="16"/>
       <c r="Z4" s="16"/>
       <c r="AA4" s="16"/>
@@ -10643,7 +10654,7 @@
   </sheetPr>
   <dimension ref="A1:AT10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="130" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="N1" zoomScale="130" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Page admin section produit
</commit_message>
<xml_diff>
--- a/Feuille_de_temps_S1-Eq1.xlsx
+++ b/Feuille_de_temps_S1-Eq1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bdebqcca-my.sharepoint.com/personal/2235096_bdeb_qc_ca/Documents/Session 4/Application Web Transanctionnelles/All-Nighter-s/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{DA9BD457-F2ED-4FC9-807C-1A231AC18EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EBB6FB4-F8BF-4190-BB85-CFEE8564723E}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{DA9BD457-F2ED-4FC9-807C-1A231AC18EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2513556-6D58-4951-8E7D-F25A52E3BEE9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -2670,8 +2670,8 @@
   </sheetPr>
   <dimension ref="A1:AE18"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="157" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2825,7 +2825,7 @@
         <v>128</v>
       </c>
       <c r="W2" s="16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X2" s="16" t="s">
         <v>142</v>
@@ -2898,7 +2898,7 @@
         <v>129</v>
       </c>
       <c r="W3" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X3" s="16" t="s">
         <v>143</v>
@@ -3246,7 +3246,7 @@
   </sheetPr>
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="O1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>

</xml_diff>